<commit_message>
updates to align with codebook review
</commit_message>
<xml_diff>
--- a/Urban-HMDA_neighborhood_data_codebook.xlsx
+++ b/Urban-HMDA_neighborhood_data_codebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26021"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="210" documentId="13_ncr:1_{BDEAD6E1-7D89-4688-BA02-ECA40F5AFA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A8E1170-C71B-453D-8E64-9180C4A563C6}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="13_ncr:1_{BDEAD6E1-7D89-4688-BA02-ECA40F5AFA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A88502D1-2F53-4033-A56F-29BF8292F5A6}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="2100" windowWidth="22860" windowHeight="13035" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Variables" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Variables!$A$1:$E$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Variables!$A$1:$H$88</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,8 +39,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={1C070B08-A698-48C8-8C88-0FBE92A04997}</author>
+    <author>Kathy Pettit</author>
+  </authors>
+  <commentList>
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{1C070B08-A698-48C8-8C88-0FBE92A04997}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    change to Native Hawaiian and Pacific Islander</t>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="1" shapeId="0" xr:uid="{38A9E1C4-273D-4CA2-B511-84816D6FB485}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Kathy Pettit:
+this was probably the right one and the AIAN purch was just mis-listed?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="279">
   <si>
     <t>Urban Institute’s Census Tract–Level Summary Files of the Home Mortgage Disclosure Act (HMDA)</t>
   </si>
@@ -92,6 +126,15 @@
     <t>Full label</t>
   </si>
   <si>
+    <t>Notes (internal)</t>
+  </si>
+  <si>
+    <t>Action Decided</t>
+  </si>
+  <si>
+    <t>Action Taken</t>
+  </si>
+  <si>
     <t>geo2010</t>
   </si>
   <si>
@@ -104,21 +147,36 @@
     <t>owner_purchase_originations</t>
   </si>
   <si>
-    <t>standard_flag</t>
-  </si>
-  <si>
     <t>Numeric</t>
   </si>
   <si>
     <t>Originations for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
+    <t>I (Will) don't believe this was included in the 2020 data; when I re-run the full file for 2021, I'll tentatively plan to include this variable, since it's the basis for so many of our other variables</t>
+  </si>
+  <si>
+    <t>More intuitive name</t>
+  </si>
+  <si>
+    <t>Renamed to 2020 variable name (owner_purchase_originations)</t>
+  </si>
+  <si>
     <t>purchase_originations</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>Originations for all first-lien home purchase originations of 1-4 unit dwellings (owner and non-owner)</t>
   </si>
   <si>
+    <t>I don't believe this was included in the 2020 data</t>
+  </si>
+  <si>
+    <t>Hold for the time being</t>
+  </si>
+  <si>
     <t>income_avail</t>
   </si>
   <si>
@@ -173,18 +231,27 @@
     <t>Originations to Hispanic borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>race_asian_purchase</t>
   </si>
   <si>
     <t>Originations to Asian borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
+    <t>I've tentatively created and added this variable (but not the corresponding race x income variables) to provide additional detail and align more directly with other datasets' racial breakdowns</t>
+  </si>
+  <si>
+    <t>Retain</t>
+  </si>
+  <si>
+    <t>Retained</t>
+  </si>
+  <si>
     <t>race_nhpi_purchase</t>
   </si>
   <si>
+    <t>Originations to Native Hawaiian and Pacific Islander borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
+  </si>
+  <si>
     <t>api_purch</t>
   </si>
   <si>
@@ -203,6 +270,9 @@
     <t>Originations to multiple race/ethnicity borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
+    <t>check code</t>
+  </si>
+  <si>
     <t>narace_purch</t>
   </si>
   <si>
@@ -230,12 +300,18 @@
     <t>Originations to American Indian/Alaskan Native borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
+    <t>Noting that the old variable names for this and the following variable were listed as the same name, though in the actual data, they were named distinctly</t>
+  </si>
+  <si>
     <t>race_asian_indian_purchase</t>
   </si>
   <si>
     <t>Originations to Asian-Indian borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
+    <t>Noting that the old variable names for this and the preceding variable were listed as the same name, though in the actual data, they were named distinctly</t>
+  </si>
+  <si>
     <t>achi_purch</t>
   </si>
   <si>
@@ -617,9 +693,21 @@
     <t>median_owner_loan_amount</t>
   </si>
   <si>
+    <t>owner_loan_amount_median</t>
+  </si>
+  <si>
     <t>Median loan amount for originations for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
+    <t>I don't believe this was provided in the 2020 data</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>Included</t>
+  </si>
+  <si>
     <t>median_loan_amount</t>
   </si>
   <si>
@@ -629,6 +717,9 @@
     <t>Median loan amount for first-lien home purchases of 1-4 unit dwellings (owner and non-owner)</t>
   </si>
   <si>
+    <t>Dropped -- I think this description was inaccurate -- this was calculated the same as the variable in row 58 ("owner_loan_amount_median")</t>
+  </si>
+  <si>
     <t>invalid_geo</t>
   </si>
   <si>
@@ -641,6 +732,9 @@
     <t>Count - 5-year 2015-2019 American Community Survey (ACS) variable (B25003_001) for total occupied housing units</t>
   </si>
   <si>
+    <t>New, ACS-derived variable</t>
+  </si>
+  <si>
     <t>occupancy_owneroccupied_count</t>
   </si>
   <si>
@@ -659,6 +753,15 @@
     <t>Originations for loans made for the purpose of investment purchases</t>
   </si>
   <si>
+    <t>New investment origination variable</t>
+  </si>
+  <si>
+    <t>change to first-lien</t>
+  </si>
+  <si>
+    <t>Limited to first-liens only</t>
+  </si>
+  <si>
     <t>occupancy_investment_units_1_4</t>
   </si>
   <si>
@@ -677,6 +780,9 @@
     <t>Originations to borrowers ages 65 and above for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
+    <t>New age purchase variable</t>
+  </si>
+  <si>
     <t>age_middleolder_purchase</t>
   </si>
   <si>
@@ -713,64 +819,100 @@
     <t>Originations for first-lien loans</t>
   </si>
   <si>
+    <t>This was called "lein1_orig" in the 2020 data, but I don't believe it was included in the codebook</t>
+  </si>
+  <si>
+    <t>Exclude</t>
+  </si>
+  <si>
+    <t>Commented out</t>
+  </si>
+  <si>
     <t>lien_subordinatelien_origination</t>
   </si>
   <si>
     <t>Originations for subordinate-lien loans</t>
   </si>
   <si>
+    <t>This was called "lein2_orig" in the 2020 data, but I don't believe it was included in the codebook</t>
+  </si>
+  <si>
     <t>purpose_purchase_origination</t>
   </si>
   <si>
     <t>Originations for loans secured for property purchases (for any number of units)</t>
   </si>
   <si>
+    <t>This was called "purch_orig" in the 2020 data, but I don't believe it was included in the codebook</t>
+  </si>
+  <si>
     <t>purpose_improvement_origination</t>
   </si>
   <si>
     <t>Originations for loans secured for property improvements (for any number of units)</t>
   </si>
   <si>
+    <t>This was called "impr_orig" in the 2020 data, but I don't believe it was included in the codebook</t>
+  </si>
+  <si>
     <t>purpose_refinance_origination</t>
   </si>
   <si>
     <t>Originations for loans secured for refinancing (for any number of units)</t>
   </si>
   <si>
+    <t>This was called "refi_orig" in the 2020 data, but I don't believe it was included in the codebook</t>
+  </si>
+  <si>
     <t>purpose_other_origination</t>
   </si>
   <si>
     <t>Originations for loans secured for other purposes (for any number of units)</t>
   </si>
   <si>
+    <t>This was called "othpurp_orig" in the 2020 data, but I don't believe it was included in the codebook</t>
+  </si>
+  <si>
     <t>race_mixed_purchase</t>
   </si>
   <si>
     <t>Originations to mixed race/ethnicity borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
+    <t>Variables for when the applicant's and co-applicant's race/ethnicity fell into diffferent categories were not included in 2020, from what I can see. Tentatively including now for consistency with the age variables, and for completeness</t>
+  </si>
+  <si>
+    <t>Confirm how these were related to variables from last year, clarify any change, confirm current year's definition, elaborate to ensure the distinction between these variables and "multiple" variables are clear</t>
+  </si>
+  <si>
+    <t>Included. Adjusted label for clarity. This variable reflects a variable that was calculated for (but not included in) the dataset for 2020. "Mixed race" refers to loan applications where: 1) there was both an applicant and a co-applicant; both applicant and co-applicant had race values provided; and the applicant and co-applicant did not have the same race value provided.</t>
+  </si>
+  <si>
     <t>race_mixed_income_verylow</t>
   </si>
   <si>
-    <t>Originations to very low-income mixed race/ethnicity borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
+    <t>Originations to very low-income mixed race/ethnicity borrowers (wherethe applicant and co-applicant belong to different race/ethnicity groups) for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
+  </si>
+  <si>
+    <t>Included. Adjusted label for clarity. This variable is new, but is based on a variable that was calculated for (but not included in) the dataset for 2020. "Mixed race" refers to loan applications where: 1) there was both an applicant and a co-applicant; both applicant and co-applicant had race values provided; and the applicant and co-applicant did not have the same race value provided.</t>
   </si>
   <si>
     <t>race_mixed_income_low</t>
   </si>
   <si>
-    <t>Originations to low-income mixed race/ethnicity borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
+    <t>Originations to low-income mixed race/ethnicity (wherethe applicant and co-applicant belong to different race/ethnicity groups) borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
     <t>race_mixed_income_moderate</t>
   </si>
   <si>
-    <t>Originations to moderate-income mixed race/ethnicity borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
+    <t>Originations to moderate-income mixed race/ethnicity (wherethe applicant and co-applicant belong to different race/ethnicity groups) borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
     <t>race_mixed_income_high</t>
   </si>
   <si>
-    <t>Originations to high-income mixed race/ethnicity borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
+    <t>Originations to high-income mixed race/ethnicity (wherethe applicant and co-applicant belong to different race/ethnicity groups) borrowers for first-lien owner-occupied home purchases of 1-4 unit dwellings</t>
   </si>
   <si>
     <t>units_1_4_origination</t>
@@ -779,10 +921,16 @@
     <t>Originations for loans for 1-4 unit dwellings</t>
   </si>
   <si>
+    <t>This was called "prop1_4_orig" in the 2020 data, but I don't believe it was included in the codebook</t>
+  </si>
+  <si>
     <t>units_5ormore_origination</t>
   </si>
   <si>
     <t>Originations for loans for dwellings with five or more units</t>
+  </si>
+  <si>
+    <t>This was called "prop5_orig" in the 2020 data, but I don't believe it was included in the codebook</t>
   </si>
 </sst>
 </file>
@@ -806,7 +954,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -816,6 +964,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,7 +986,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -845,6 +999,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,6 +1017,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Kathy Pettit" id="{F335753E-9046-4BA4-A05C-D4388CAD3EA4}" userId="" providerId=""/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1157,6 +1320,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E12" dT="2023-01-12T18:38:02.85" personId="{F335753E-9046-4BA4-A05C-D4388CAD3EA4}" id="{1C070B08-A698-48C8-8C88-0FBE92A04997}">
+    <text>change to Native Hawaiian and Pacific Islander</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A7"/>
@@ -1200,12 +1371,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E88"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M86" sqref="M86"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1214,9 +1385,11 @@
     <col min="2" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="58.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" customWidth="1"/>
+    <col min="7" max="8" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1232,523 +1405,577 @@
       <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30.75">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30.75">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30.75">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30.75">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30.75">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30.75">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30.75">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30.75">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="29.25" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="29.25" customHeight="1">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30.75">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30.75">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30.75">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30.75">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30.75">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30.75">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30.75">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30.75">
       <c r="B11" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30.75">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30.75">
       <c r="B12" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45.75">
+        <v>17</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45.75">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30.75">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30.75">
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
-        <v>44</v>
+      <c r="B14" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30.75">
+        <v>57</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30.75">
       <c r="A15">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30.75">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30.75">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30.75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30.75">
       <c r="A17">
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30.75">
+        <v>67</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30.75">
       <c r="A18">
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30.75">
+        <v>70</v>
+      </c>
+      <c r="F18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30.75">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30.75">
       <c r="A20">
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30.75">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30.75">
       <c r="A21">
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30.75">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30.75">
       <c r="A22">
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30.75">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30.75">
       <c r="A23">
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30.75">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30.75">
       <c r="A24">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30.75">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30.75">
       <c r="A25">
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30.75">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30.75">
       <c r="A26">
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30.75">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30.75">
       <c r="A27">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30.75">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30.75">
       <c r="A28">
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30.75">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30.75">
       <c r="A29">
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30.75">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30.75">
       <c r="A30">
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30.75">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30.75">
       <c r="A31">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30.75">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30.75">
       <c r="A32">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30.75">
@@ -1756,16 +1983,16 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30.75">
@@ -1773,16 +2000,16 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30.75">
@@ -1790,16 +2017,16 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30.75">
@@ -1807,16 +2034,16 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30.75">
@@ -1824,16 +2051,16 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="C37" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="30.75">
@@ -1841,16 +2068,16 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="D38" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="30.75">
@@ -1858,16 +2085,16 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="45.75">
@@ -1875,16 +2102,16 @@
         <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="C40" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="45.75">
@@ -1892,16 +2119,16 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="C41" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="45.75">
@@ -1909,16 +2136,16 @@
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="C42" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="D42" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="45.75">
@@ -1926,16 +2153,16 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="C43" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="D43" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="45.75">
@@ -1943,16 +2170,16 @@
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="45.75">
@@ -1960,16 +2187,16 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="C45" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D45" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="45.75">
@@ -1977,16 +2204,16 @@
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C46" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="D46" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="45.75">
@@ -1994,16 +2221,16 @@
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="D47" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="30.75">
@@ -2011,623 +2238,811 @@
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="C48" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30.75">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="30.75">
       <c r="A49">
         <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="D49" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="36.75" customHeight="1">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="36.75" customHeight="1">
       <c r="A50">
         <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D50" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="30.75">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="30.75">
       <c r="A51">
         <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="C51" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30.75">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="30.75">
       <c r="A52">
         <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="C52" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="D52" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="30.75">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="30.75">
       <c r="A53">
         <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="C53" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="D53" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30.75">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="30.75">
       <c r="A54">
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="C54" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="D54" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30.75">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="30.75">
       <c r="A55">
         <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="C55" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30.75">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="30.75">
       <c r="A56">
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="C56" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="D56" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="30.75">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="30.75">
       <c r="A57">
         <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="C57" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="D57" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="30.75">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="30.75">
       <c r="A58">
         <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="C58" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="D58" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="30.75">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="30.75">
       <c r="A59">
         <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="C59" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="30.75">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="30.75">
       <c r="A60">
         <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="C60" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="D60" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="30.75">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="30.75">
       <c r="A61">
         <v>58</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>184</v>
+        <v>198</v>
+      </c>
+      <c r="C61" t="s">
+        <v>199</v>
       </c>
       <c r="D61" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="30.75">
+        <v>200</v>
+      </c>
+      <c r="F61" t="s">
+        <v>201</v>
+      </c>
+      <c r="G61" t="s">
+        <v>202</v>
+      </c>
+      <c r="H61" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="30.75">
       <c r="A62">
         <v>59</v>
       </c>
-      <c r="B62" t="s">
-        <v>186</v>
+      <c r="B62" s="5" t="s">
+        <v>204</v>
       </c>
       <c r="C62" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="D62" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>206</v>
+      </c>
+      <c r="H62" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="C63" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="D63" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="30.75">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="30.75">
       <c r="B64" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C64" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="D64" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="30.75">
+        <v>211</v>
+      </c>
+      <c r="F64" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" ht="30.75">
       <c r="B65" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C65" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="D65" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" ht="45.75">
+        <v>214</v>
+      </c>
+      <c r="F65" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="45.75">
       <c r="B66" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C66" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="D66" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" ht="30.75">
+        <v>216</v>
+      </c>
+      <c r="F66" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" ht="30.75">
       <c r="B67" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C67" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="D67" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" ht="30.75">
+        <v>218</v>
+      </c>
+      <c r="F67" t="s">
+        <v>219</v>
+      </c>
+      <c r="G67" t="s">
+        <v>220</v>
+      </c>
+      <c r="H67" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" ht="30.75">
       <c r="B68" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C68" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="D68" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" ht="30.75">
+        <v>223</v>
+      </c>
+      <c r="F68" t="s">
+        <v>219</v>
+      </c>
+      <c r="G68" t="s">
+        <v>220</v>
+      </c>
+      <c r="H68" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" ht="30.75">
       <c r="B69" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C69" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
       <c r="D69" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" ht="30.75">
+        <v>225</v>
+      </c>
+      <c r="F69" t="s">
+        <v>219</v>
+      </c>
+      <c r="G69" t="s">
+        <v>220</v>
+      </c>
+      <c r="H69" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" ht="30.75">
       <c r="B70" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C70" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="D70" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" ht="30.75">
+        <v>227</v>
+      </c>
+      <c r="F70" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="30.75">
       <c r="B71" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C71" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="D71" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" ht="30.75">
+        <v>230</v>
+      </c>
+      <c r="F71" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" ht="30.75">
       <c r="B72" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C72" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="D72" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" ht="30.75">
+        <v>232</v>
+      </c>
+      <c r="F72" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" ht="30.75">
       <c r="B73" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C73" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="D73" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" ht="45.75">
+        <v>234</v>
+      </c>
+      <c r="F73" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" ht="45.75">
       <c r="B74" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C74" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="D74" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" ht="30.75">
+        <v>236</v>
+      </c>
+      <c r="F74" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" ht="30.75">
       <c r="B75" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C75" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="D75" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5">
+        <v>238</v>
+      </c>
+      <c r="F75" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8">
       <c r="B76" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C76" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="D76" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5">
+        <v>240</v>
+      </c>
+      <c r="F76" t="s">
+        <v>241</v>
+      </c>
+      <c r="G76" t="s">
+        <v>242</v>
+      </c>
+      <c r="H76" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8">
       <c r="B77" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C77" t="s">
-        <v>217</v>
+        <v>244</v>
       </c>
       <c r="D77" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" ht="30.75">
+        <v>245</v>
+      </c>
+      <c r="F77" t="s">
+        <v>246</v>
+      </c>
+      <c r="G77" t="s">
+        <v>242</v>
+      </c>
+      <c r="H77" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" ht="30.75">
       <c r="B78" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C78" t="s">
-        <v>219</v>
+        <v>247</v>
       </c>
       <c r="D78" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" ht="30.75">
+        <v>248</v>
+      </c>
+      <c r="F78" t="s">
+        <v>249</v>
+      </c>
+      <c r="G78" t="s">
+        <v>242</v>
+      </c>
+      <c r="H78" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" ht="30.75">
       <c r="B79" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C79" t="s">
-        <v>221</v>
+        <v>250</v>
       </c>
       <c r="D79" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" ht="30.75">
+        <v>251</v>
+      </c>
+      <c r="F79" t="s">
+        <v>252</v>
+      </c>
+      <c r="G79" t="s">
+        <v>242</v>
+      </c>
+      <c r="H79" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" ht="30.75">
       <c r="B80" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C80" t="s">
-        <v>223</v>
+        <v>253</v>
       </c>
       <c r="D80" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" ht="30.75">
+        <v>254</v>
+      </c>
+      <c r="F80" t="s">
+        <v>255</v>
+      </c>
+      <c r="G80" t="s">
+        <v>242</v>
+      </c>
+      <c r="H80" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" ht="30.75">
       <c r="B81" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C81" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
       <c r="D81" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" ht="30.75">
+        <v>257</v>
+      </c>
+      <c r="F81" t="s">
+        <v>258</v>
+      </c>
+      <c r="G81" t="s">
+        <v>242</v>
+      </c>
+      <c r="H81" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" ht="30.75">
       <c r="B82" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C82" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="D82" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" ht="30.75">
+        <v>260</v>
+      </c>
+      <c r="F82" t="s">
+        <v>261</v>
+      </c>
+      <c r="G82" t="s">
+        <v>262</v>
+      </c>
+      <c r="H82" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" ht="60.75">
       <c r="B83" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C83" t="s">
-        <v>229</v>
+        <v>264</v>
       </c>
       <c r="D83" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" ht="30.75">
+        <v>265</v>
+      </c>
+      <c r="F83" t="s">
+        <v>261</v>
+      </c>
+      <c r="G83" t="s">
+        <v>262</v>
+      </c>
+      <c r="H83" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" ht="60.75">
       <c r="B84" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C84" t="s">
-        <v>231</v>
+        <v>267</v>
       </c>
       <c r="D84" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" ht="30.75">
+        <v>268</v>
+      </c>
+      <c r="F84" t="s">
+        <v>261</v>
+      </c>
+      <c r="G84" t="s">
+        <v>262</v>
+      </c>
+      <c r="H84" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" ht="60.75">
       <c r="B85" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C85" t="s">
-        <v>233</v>
+        <v>269</v>
       </c>
       <c r="D85" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" ht="30.75">
+        <v>270</v>
+      </c>
+      <c r="F85" t="s">
+        <v>261</v>
+      </c>
+      <c r="G85" t="s">
+        <v>262</v>
+      </c>
+      <c r="H85" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" ht="60.75">
       <c r="B86" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C86" t="s">
-        <v>235</v>
+        <v>271</v>
       </c>
       <c r="D86" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5">
+        <v>272</v>
+      </c>
+      <c r="F86" t="s">
+        <v>261</v>
+      </c>
+      <c r="G86" t="s">
+        <v>262</v>
+      </c>
+      <c r="H86" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8">
       <c r="B87" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C87" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
       <c r="D87" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5">
+        <v>274</v>
+      </c>
+      <c r="F87" t="s">
+        <v>275</v>
+      </c>
+      <c r="G87" t="s">
+        <v>242</v>
+      </c>
+      <c r="H87" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8">
       <c r="B88" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C88" t="s">
-        <v>239</v>
+        <v>276</v>
       </c>
       <c r="D88" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>240</v>
+        <v>277</v>
+      </c>
+      <c r="F88" t="s">
+        <v>278</v>
+      </c>
+      <c r="G88" t="s">
+        <v>242</v>
+      </c>
+      <c r="H88" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H88" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>